<commit_message>
Atualização do relatório finalizada
</commit_message>
<xml_diff>
--- a/relatorio_projetos.xlsx
+++ b/relatorio_projetos.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,27 +422,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nome da Ferramenta</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Projeto</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Técnico</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>IDGEO</t>
         </is>
@@ -463,32 +451,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HASTE DE INJEÇÃO</t>
+          <t>HOLLOW PARAFUSO 1,5M</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>VOLKS</t>
+          <t>VOLKSWAGEN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AMAURI</t>
+          <t>NELSON</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SP24001</t>
+          <t>SP24009</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PROBE BIPARTIDO</t>
+          <t>PROBE</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -496,7 +484,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CSN</t>
+          <t>SP25001</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -507,6 +495,56 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>RJ23001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HASTE INJEÇÃO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SP25001</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AMAURI</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RJ23001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HASTE INJEÇÃO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>VOLKSWAGEN</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NELSON</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SP24009</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Programa funcionando e com servidor
</commit_message>
<xml_diff>
--- a/relatorio_projetos.xlsx
+++ b/relatorio_projetos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,11 +456,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HASTE INOX 1M</t>
+          <t>PONTEIRA FIXA INOX</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -486,11 +486,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PONTEIRA FIXA INOX</t>
+          <t>BOMBA PNEUMATICA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BOMBA PNEUMATICA</t>
+          <t>TE DE INJEÇÃO</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -546,11 +546,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TE DE INJEÇÃO</t>
+          <t>MISTURADOR</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -576,11 +576,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MISTURADOR</t>
+          <t>HASTE HELICOIDAL 6" 1,5M</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -589,28 +589,28 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>QUALITA</t>
+          <t>VLI</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>AMAURI / THIAGO SILVA</t>
+          <t>EDUARDO RIBEIRO</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>PR24045</t>
+          <t>BA25002</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T INOX COM SAIDA MANOMETRO</t>
+          <t>PONTEIRA TRICONICA 6"</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -619,28 +619,28 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>QUALITA</t>
+          <t>VLI</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AMAURI / THIAGO SILVA</t>
+          <t>EDUARDO RIBEIRO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>PR24045</t>
+          <t>BA25002</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SACADOR DE HASTE</t>
+          <t>PONTEIRA HELICOIDAL 6" 1M</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -649,45 +649,285 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>QUALITA</t>
+          <t>VLI</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>AMAURI / THIAGO SILVA</t>
+          <t>EDUARDO RIBEIRO</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>PR24045</t>
+          <t>BA25002</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>HASTE INJEÇÃO 1,2M</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ADAPTADOR PROBE MACHO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ADAPTADOR PROBE FEMEA</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SACADOR DE HASTE </t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EXTRATOR DE HASTE</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SACADOR DE HASTE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>QUALITA</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>AMAURI / THIAGO SILVA</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>PR24045</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>BATEDOR</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>VLI</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>EDUARDO RIBEIRO</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>BA25002</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BATEDOR</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>1</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>uso</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>QUALITA</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>AMAURI / THIAGO SILVA</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>PR24045</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HASTE INOX 1M</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>25</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>uso</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>QUALITA</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>AMAURI / THIAGO SILVA</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>PR24045</t>
         </is>

</xml_diff>